<commit_message>
midway through storm 3
</commit_message>
<xml_diff>
--- a/LakeHodges/Rating Curve and Pacings Development/Hodges Creeks pacing worksheet - Storm 1.xlsx
+++ b/LakeHodges/Rating Curve and Pacings Development/Hodges Creeks pacing worksheet - Storm 1.xlsx
@@ -240,6 +240,7 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="3" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -249,7 +250,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -626,7 +626,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
@@ -667,7 +667,7 @@
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="13" t="s">
         <v>7</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -710,7 +710,7 @@
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A3" s="13"/>
+      <c r="A3" s="14"/>
       <c r="B3" s="3" t="s">
         <v>10</v>
       </c>
@@ -730,7 +730,7 @@
       </c>
     </row>
     <row r="4" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="14"/>
+      <c r="A4" s="15"/>
       <c r="B4" s="4" t="s">
         <v>2</v>
       </c>
@@ -750,7 +750,7 @@
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A5" s="12" t="s">
+      <c r="A5" s="13" t="s">
         <v>8</v>
       </c>
       <c r="B5" s="2" t="s">
@@ -775,7 +775,7 @@
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A6" s="13"/>
+      <c r="A6" s="14"/>
       <c r="B6" s="3" t="s">
         <v>10</v>
       </c>
@@ -795,7 +795,7 @@
       </c>
     </row>
     <row r="7" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="14"/>
+      <c r="A7" s="15"/>
       <c r="B7" s="4" t="s">
         <v>2</v>
       </c>
@@ -815,7 +815,7 @@
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A8" s="12" t="s">
+      <c r="A8" s="13" t="s">
         <v>11</v>
       </c>
       <c r="B8" s="2" t="s">
@@ -846,7 +846,7 @@
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A9" s="13"/>
+      <c r="A9" s="14"/>
       <c r="B9" s="3" t="s">
         <v>10</v>
       </c>
@@ -869,7 +869,7 @@
       </c>
     </row>
     <row r="10" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="13"/>
+      <c r="A10" s="14"/>
       <c r="B10" s="3" t="s">
         <v>2</v>
       </c>
@@ -889,7 +889,7 @@
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A11" s="12" t="s">
+      <c r="A11" s="13" t="s">
         <v>9</v>
       </c>
       <c r="B11" s="2" t="s">
@@ -904,7 +904,7 @@
       <c r="E11" s="2">
         <v>1650</v>
       </c>
-      <c r="F11" s="15">
+      <c r="F11" s="12">
         <f>D11*60*5*0.6</f>
         <v>990</v>
       </c>
@@ -913,7 +913,7 @@
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A12" s="13"/>
+      <c r="A12" s="14"/>
       <c r="B12" s="3" t="s">
         <v>1</v>
       </c>
@@ -927,7 +927,7 @@
         <f>D12*60*5</f>
         <v>25800</v>
       </c>
-      <c r="F12" s="15">
+      <c r="F12" s="12">
         <f>D12*60*5*0.6</f>
         <v>15480</v>
       </c>
@@ -939,7 +939,7 @@
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A13" s="13"/>
+      <c r="A13" s="14"/>
       <c r="B13" s="3" t="s">
         <v>10</v>
       </c>
@@ -955,7 +955,7 @@
       </c>
     </row>
     <row r="14" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="14"/>
+      <c r="A14" s="15"/>
       <c r="B14" s="4" t="s">
         <v>2</v>
       </c>
@@ -971,7 +971,7 @@
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A15" s="12" t="s">
+      <c r="A15" s="13" t="s">
         <v>12</v>
       </c>
       <c r="B15" s="2" t="s">
@@ -996,7 +996,7 @@
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A16" s="13"/>
+      <c r="A16" s="14"/>
       <c r="B16" s="3" t="s">
         <v>10</v>
       </c>
@@ -1016,7 +1016,7 @@
       </c>
     </row>
     <row r="17" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="14"/>
+      <c r="A17" s="15"/>
       <c r="B17" s="4" t="s">
         <v>2</v>
       </c>
@@ -1036,7 +1036,7 @@
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A18" s="12" t="s">
+      <c r="A18" s="13" t="s">
         <v>13</v>
       </c>
       <c r="B18" s="2" t="s">
@@ -1061,7 +1061,7 @@
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A19" s="13"/>
+      <c r="A19" s="14"/>
       <c r="B19" s="3" t="s">
         <v>10</v>
       </c>
@@ -1081,7 +1081,7 @@
       </c>
     </row>
     <row r="20" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="14"/>
+      <c r="A20" s="15"/>
       <c r="B20" s="4" t="s">
         <v>2</v>
       </c>
@@ -1101,7 +1101,7 @@
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A21" s="12" t="s">
+      <c r="A21" s="13" t="s">
         <v>14</v>
       </c>
       <c r="B21" s="2" t="s">
@@ -1132,7 +1132,7 @@
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A22" s="13"/>
+      <c r="A22" s="14"/>
       <c r="B22" s="3" t="s">
         <v>10</v>
       </c>
@@ -1152,7 +1152,7 @@
       </c>
     </row>
     <row r="23" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="14"/>
+      <c r="A23" s="15"/>
       <c r="B23" s="4" t="s">
         <v>2</v>
       </c>
@@ -1172,7 +1172,7 @@
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A24" s="12" t="s">
+      <c r="A24" s="13" t="s">
         <v>15</v>
       </c>
       <c r="B24" s="2" t="s">
@@ -1203,7 +1203,7 @@
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A25" s="13"/>
+      <c r="A25" s="14"/>
       <c r="B25" s="3" t="s">
         <v>1</v>
       </c>
@@ -1217,14 +1217,14 @@
         <f t="shared" ref="E25" si="3">D25*60*5</f>
         <v>108846</v>
       </c>
-      <c r="F25" s="15">
+      <c r="F25" s="12">
         <f t="shared" ref="F25" si="4">D25*60*5*0.6</f>
         <v>65307.6</v>
       </c>
       <c r="G25" s="11"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A26" s="13"/>
+      <c r="A26" s="14"/>
       <c r="B26" s="3" t="s">
         <v>10</v>
       </c>
@@ -1244,7 +1244,7 @@
       </c>
     </row>
     <row r="27" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="14"/>
+      <c r="A27" s="15"/>
       <c r="B27" s="4" t="s">
         <v>2</v>
       </c>
@@ -1264,7 +1264,7 @@
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A28" s="12" t="s">
+      <c r="A28" s="13" t="s">
         <v>16</v>
       </c>
       <c r="B28" s="2" t="s">
@@ -1295,7 +1295,7 @@
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A29" s="13"/>
+      <c r="A29" s="14"/>
       <c r="B29" s="3" t="s">
         <v>1</v>
       </c>
@@ -1309,14 +1309,14 @@
         <f t="shared" ref="E29" si="5">D29*60*5</f>
         <v>22712.999999999996</v>
       </c>
-      <c r="F29" s="15">
+      <c r="F29" s="12">
         <f t="shared" ref="F29" si="6">D29*60*5*0.6</f>
         <v>13627.799999999997</v>
       </c>
       <c r="G29" s="11"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A30" s="13"/>
+      <c r="A30" s="14"/>
       <c r="B30" s="3" t="s">
         <v>10</v>
       </c>
@@ -1336,7 +1336,7 @@
       </c>
     </row>
     <row r="31" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="14"/>
+      <c r="A31" s="15"/>
       <c r="B31" s="4" t="s">
         <v>2</v>
       </c>

</xml_diff>